<commit_message>
Ajuste na base enviar
</commit_message>
<xml_diff>
--- a/Enviar.xlsx
+++ b/Enviar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bulllasa-my.sharepoint.com/personal/gabriel_souza_bullla_com_br/Documents/ws-hashtag-programacao/aut_envio_msg_whatsapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="14_{23ED55AB-1320-4A4F-9F43-C5D3D0631604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA910393-7022-4300-A52B-AA73A4277E05}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="14_{23ED55AB-1320-4A4F-9F43-C5D3D0631604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF9C2111-5AED-4B64-8B6B-F3157894A671}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18810" windowHeight="15750" xr2:uid="{F81C85CE-3BCD-4B33-8C8B-0A39913C8743}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Pessoa</t>
   </si>
@@ -49,16 +49,13 @@
     <t>Oi, isso é uma mensagem de teste (:</t>
   </si>
   <si>
-    <t>5511962760649</t>
-  </si>
-  <si>
     <t>João</t>
   </si>
   <si>
     <t>Luis</t>
   </si>
   <si>
-    <t>5511940337691</t>
+    <t>Digite seu número</t>
   </si>
 </sst>
 </file>
@@ -416,7 +413,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,10 +436,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -450,10 +447,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>

</xml_diff>